<commit_message>
add undergraduate to 2 charts titles, numbered spreadsheet tabs
</commit_message>
<xml_diff>
--- a/data/DataforDownload.xlsx
+++ b/data/DataforDownload.xlsx
@@ -4,46 +4,46 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="821"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="43920" windowHeight="26360" tabRatio="821"/>
   </bookViews>
   <sheets>
-    <sheet name="Enroll.TwoYear" sheetId="6" r:id="rId1"/>
-    <sheet name="Enroll.Migration" sheetId="7" r:id="rId2"/>
-    <sheet name="Enroll.Change" sheetId="8" r:id="rId3"/>
-    <sheet name="Fund.Income" sheetId="9" r:id="rId4"/>
-    <sheet name="Fund.GrantAid" sheetId="10" r:id="rId5"/>
-    <sheet name="Fund.TotalChange" sheetId="11" r:id="rId6"/>
-    <sheet name="Fund.PerStudent" sheetId="12" r:id="rId7"/>
-    <sheet name="Tuition.Change" sheetId="13" r:id="rId8"/>
-    <sheet name="Tuition.Tuition&amp;Rank" sheetId="14" r:id="rId9"/>
-    <sheet name="Annual Data" sheetId="1" r:id="rId10"/>
-    <sheet name="Nonannual Data" sheetId="2" r:id="rId11"/>
-    <sheet name="Sources" sheetId="3" r:id="rId12"/>
-    <sheet name="NCES Enrollment Source Detail" sheetId="4" r:id="rId13"/>
-    <sheet name="Grapevine Source Detail" sheetId="5" r:id="rId14"/>
+    <sheet name="1 Enroll.TwoYear" sheetId="6" r:id="rId1"/>
+    <sheet name="2 Enroll.Migration" sheetId="7" r:id="rId2"/>
+    <sheet name="3 Enroll.Change" sheetId="8" r:id="rId3"/>
+    <sheet name="4 Fund.Income" sheetId="9" r:id="rId4"/>
+    <sheet name="5 Fund.GrantAid" sheetId="10" r:id="rId5"/>
+    <sheet name="6 Fund.TotalChange" sheetId="11" r:id="rId6"/>
+    <sheet name="7 Fund.PerStudent" sheetId="12" r:id="rId7"/>
+    <sheet name="8 Tuition.Change" sheetId="13" r:id="rId8"/>
+    <sheet name="9 Tuition.Tuition&amp;Rank" sheetId="14" r:id="rId9"/>
+    <sheet name="10 Annual Data" sheetId="1" r:id="rId10"/>
+    <sheet name="11 Nonannual Data" sheetId="2" r:id="rId11"/>
+    <sheet name="12 Sources" sheetId="3" r:id="rId12"/>
+    <sheet name="13 NCES Enrollment SourceDetail" sheetId="4" r:id="rId13"/>
+    <sheet name="14 Grapevine Source Detail" sheetId="5" r:id="rId14"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId15"/>
     <externalReference r:id="rId16"/>
   </externalReferences>
   <definedNames>
+    <definedName name="currentdollars" localSheetId="0">'[1]Total appropriations'!$B$2:$P$2</definedName>
+    <definedName name="currentdollars" localSheetId="1">'[1]Total appropriations'!$B$2:$P$2</definedName>
     <definedName name="currentdollars" localSheetId="2">'[1]Total appropriations'!$B$2:$P$2</definedName>
-    <definedName name="currentdollars" localSheetId="1">'[1]Total appropriations'!$B$2:$P$2</definedName>
-    <definedName name="currentdollars" localSheetId="0">'[1]Total appropriations'!$B$2:$P$2</definedName>
+    <definedName name="currentdollars" localSheetId="3">'[1]Total appropriations'!$B$2:$P$2</definedName>
     <definedName name="currentdollars" localSheetId="4">'[1]Total appropriations'!$B$2:$P$2</definedName>
-    <definedName name="currentdollars" localSheetId="3">'[1]Total appropriations'!$B$2:$P$2</definedName>
+    <definedName name="currentdollars" localSheetId="5">'[1]Total appropriations'!$B$2:$P$2</definedName>
     <definedName name="currentdollars" localSheetId="6">'[1]Total appropriations'!$B$2:$P$2</definedName>
-    <definedName name="currentdollars" localSheetId="5">'[1]Total appropriations'!$B$2:$P$2</definedName>
     <definedName name="currentdollars" localSheetId="7">'[1]Total appropriations'!$B$2:$P$2</definedName>
     <definedName name="currentdollars" localSheetId="8">'[1]Total appropriations'!$B$2:$P$2</definedName>
     <definedName name="currentdollars">'[2]Total appropriations'!$B$2:$P$2</definedName>
+    <definedName name="real" localSheetId="0">'[1]Total appropriations'!$B$3:$P$3</definedName>
+    <definedName name="real" localSheetId="1">'[1]Total appropriations'!$B$3:$P$3</definedName>
     <definedName name="real" localSheetId="2">'[1]Total appropriations'!$B$3:$P$3</definedName>
-    <definedName name="real" localSheetId="1">'[1]Total appropriations'!$B$3:$P$3</definedName>
-    <definedName name="real" localSheetId="0">'[1]Total appropriations'!$B$3:$P$3</definedName>
+    <definedName name="real" localSheetId="3">'[1]Total appropriations'!$B$3:$P$3</definedName>
     <definedName name="real" localSheetId="4">'[1]Total appropriations'!$B$3:$P$3</definedName>
-    <definedName name="real" localSheetId="3">'[1]Total appropriations'!$B$3:$P$3</definedName>
+    <definedName name="real" localSheetId="5">'[1]Total appropriations'!$B$3:$P$3</definedName>
     <definedName name="real" localSheetId="6">'[1]Total appropriations'!$B$3:$P$3</definedName>
-    <definedName name="real" localSheetId="5">'[1]Total appropriations'!$B$3:$P$3</definedName>
     <definedName name="real" localSheetId="7">'[1]Total appropriations'!$B$3:$P$3</definedName>
     <definedName name="real" localSheetId="8">'[1]Total appropriations'!$B$3:$P$3</definedName>
     <definedName name="real">'[2]Total appropriations'!$B$3:$P$3</definedName>
@@ -489,25 +489,7 @@
     <t>description</t>
   </si>
   <si>
-    <t>State Funding for Higher Education per $1,000 in Personal Income, 2014-15</t>
-  </si>
-  <si>
     <t>source</t>
-  </si>
-  <si>
-    <t>Percentage of FTE Public Enrollments in Two-Year Colleges, by State, Fall 2012</t>
-  </si>
-  <si>
-    <t>Undergraduate Grant Dollars per Undergraduate FTE</t>
-  </si>
-  <si>
-    <t>Percent of Undergraduate Grant Dollars that are Need-Based</t>
-  </si>
-  <si>
-    <t>Need-based Undergraduate Grant Dollars per Undergraduate FTE</t>
-  </si>
-  <si>
-    <t>Non-need-based Undergraduate Grant Dollars per Undergraduate FTE</t>
   </si>
   <si>
     <t>https://www.nassgap.org/viewrepository.aspx?categoryID=3#</t>
@@ -918,9 +900,6 @@
     <t>https://nces.ed.gov/programs/digest/d13/tables/dt13_309.20.asp</t>
   </si>
   <si>
-    <t>Enrollment Chart 1. Share of Public Enrollment in Two-Year Institutions, Fall 2012</t>
-  </si>
-  <si>
     <t>Enrollment in two-year institutions</t>
   </si>
   <si>
@@ -1135,9 +1114,6 @@
       </rPr>
       <t xml:space="preserve"> Fall 2014 FTE student enrollment estimates are based on fall 2013 enrollment by state, updated with the NCES predicted increase of 0.03 percent for the nation as a whole; Personal income data are for the second quarter of 2014.</t>
     </r>
-  </si>
-  <si>
-    <t>Enrollment Chart 2. State Grant Aid to Students: Need Based versus Non-Need Based, Fall 2013</t>
   </si>
   <si>
     <t>State grant aid per student</t>
@@ -1417,6 +1393,30 @@
       </rPr>
       <t xml:space="preserve"> Tuition data are in-district tuition for public two-year and in-state tuition for public four-year colleges. Average tuition and fee prices are weighted by full-time enrollment. Data on individual states should be interpreted with caution because of the possible impact of reporting errors and missing data on states with small numbers of institutions. Only public four-year tuition and fees are shown for Alaska because this state does not have a community college system.</t>
     </r>
+  </si>
+  <si>
+    <t>Enrollment Chart 2. State Grant Aid to Undergraduate Students: Need Based versus Non-Need Based, Fall 2013</t>
+  </si>
+  <si>
+    <t>Enrollment Chart 1. Share of Public Undergraduate Enrollment in Two-Year Institutions, Fall 2012</t>
+  </si>
+  <si>
+    <t>Percentage of FTE public undergraduate enrollments in two-year colleges, by state, Fall 2012</t>
+  </si>
+  <si>
+    <t>Undergraduate grant dollars per undergraduate FTE</t>
+  </si>
+  <si>
+    <t>Percent of undergraduate grant dollars that are need-based</t>
+  </si>
+  <si>
+    <t>Need-based undergraduate grant dollars per undergraduate FTE</t>
+  </si>
+  <si>
+    <t>Non-need-based undergraduate grant dollars per undergraduate FTE</t>
+  </si>
+  <si>
+    <t>State funding for higher education per $1,000 in personal income, 2014-15</t>
   </si>
 </sst>
 </file>
@@ -3182,7 +3182,7 @@
   <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3192,7 +3192,7 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="82" t="s">
-        <v>255</v>
+        <v>289</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -3201,13 +3201,13 @@
     <row r="2" spans="1:4" ht="34" customHeight="1">
       <c r="A2" s="40"/>
       <c r="B2" s="41" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="C2" s="41" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D2" s="42" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3243,13 +3243,13 @@
         <v>13</v>
       </c>
       <c r="B5" s="44" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C5" s="44">
         <v>20318</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3926,7 +3926,7 @@
     </row>
     <row r="54" spans="1:4" ht="63" customHeight="1">
       <c r="A54" s="85" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B54" s="86"/>
       <c r="C54" s="86"/>
@@ -3981,7 +3981,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="E1" s="27" t="s">
         <v>3</v>
@@ -32227,8 +32227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -36747,7 +36747,7 @@
   <sheetData>
     <row r="1" spans="1:6" s="15" customFormat="1">
       <c r="A1" s="15" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>138</v>
@@ -36756,622 +36756,622 @@
         <v>139</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="D8" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>113</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>140</v>
+        <v>295</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>142</v>
+        <v>290</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>115</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>143</v>
+        <v>291</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>144</v>
+        <v>292</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>117</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>145</v>
+        <v>293</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>118</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>146</v>
+        <v>294</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>119</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>120</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>121</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>123</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>125</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>197</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>132</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>133</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="1" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>134</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="E33" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="E34" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>192</v>
-      </c>
       <c r="E35" s="1" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="1" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -37401,9 +37401,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
@@ -37416,24 +37414,24 @@
   <sheetData>
     <row r="1" spans="1:5" s="16" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="17" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B2" s="17">
         <v>2004</v>
@@ -37445,7 +37443,7 @@
         <v>36799</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -37462,12 +37460,12 @@
         <v>37225</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="17" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="B4" s="17">
         <v>2006</v>
@@ -37479,12 +37477,12 @@
         <v>37468</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="17" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B5" s="17">
         <v>2009</v>
@@ -37496,7 +37494,7 @@
         <v>38533</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -37513,7 +37511,7 @@
         <v>38837</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -37530,7 +37528,7 @@
         <v>39386</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -37547,12 +37545,12 @@
         <v>39691</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="17" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="B9" s="17">
         <v>2013</v>
@@ -37564,7 +37562,7 @@
         <v>40209</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -37581,12 +37579,12 @@
         <v>40482</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="17" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="B11" s="17">
         <v>2014</v>
@@ -37598,7 +37596,7 @@
         <v>40602</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>
@@ -37615,9 +37613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
@@ -37629,13 +37625,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="16" customFormat="1">
       <c r="A1" s="16" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -37643,43 +37639,43 @@
         <v>2001</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="7" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -37687,10 +37683,10 @@
         <v>2010</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -37698,10 +37694,10 @@
         <v>2011</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -37709,21 +37705,21 @@
         <v>2012</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="7" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -37751,7 +37747,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="82" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="84"/>
@@ -37759,10 +37755,10 @@
     <row r="2" spans="1:6" ht="37" customHeight="1">
       <c r="A2" s="49"/>
       <c r="B2" s="41" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -38329,7 +38325,7 @@
     </row>
     <row r="54" spans="1:3" ht="38.25" customHeight="1">
       <c r="A54" s="88" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="B54" s="89"/>
       <c r="C54" s="90"/>
@@ -38364,7 +38360,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" s="82" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -40825,7 +40821,7 @@
     </row>
     <row r="54" spans="1:15" ht="16" customHeight="1">
       <c r="A54" s="82" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="B54" s="83"/>
       <c r="C54" s="83"/>
@@ -43286,7 +43282,7 @@
     </row>
     <row r="107" spans="1:15" ht="40.5" customHeight="1">
       <c r="A107" s="88" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="B107" s="89"/>
       <c r="C107" s="89"/>
@@ -43334,7 +43330,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="82" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="84"/>
@@ -43342,10 +43338,10 @@
     <row r="2" spans="1:6">
       <c r="A2" s="49"/>
       <c r="B2" s="41" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -43912,7 +43908,7 @@
     </row>
     <row r="54" spans="1:3" ht="80.25" customHeight="1">
       <c r="A54" s="88" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B54" s="89"/>
       <c r="C54" s="90"/>
@@ -43947,7 +43943,7 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="82" t="s">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -43957,24 +43953,24 @@
     <row r="2" spans="1:8">
       <c r="A2" s="62"/>
       <c r="B2" s="92" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C2" s="83"/>
       <c r="D2" s="84"/>
       <c r="E2" s="93" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="63"/>
       <c r="B3" s="41" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="E3" s="94"/>
     </row>
@@ -44515,7 +44511,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -44898,7 +44894,7 @@
     </row>
     <row r="55" spans="1:5" ht="60" customHeight="1">
       <c r="A55" s="88" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="B55" s="89"/>
       <c r="C55" s="89"/>
@@ -44937,7 +44933,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16" customHeight="1">
       <c r="A1" s="82" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -47555,7 +47551,7 @@
     </row>
     <row r="54" spans="1:16" ht="16" customHeight="1">
       <c r="A54" s="82" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="B54" s="83"/>
       <c r="C54" s="83"/>
@@ -50173,7 +50169,7 @@
     </row>
     <row r="107" spans="1:16" ht="42.75" customHeight="1">
       <c r="A107" s="88" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="B107" s="89"/>
       <c r="C107" s="89"/>
@@ -50222,7 +50218,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="16" customHeight="1">
       <c r="A1" s="82" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -50285,7 +50281,7 @@
         <v>2014</v>
       </c>
       <c r="P2" s="68" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:16">
@@ -52840,7 +52836,7 @@
     </row>
     <row r="54" spans="1:16" ht="63" customHeight="1">
       <c r="A54" s="88" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="B54" s="89"/>
       <c r="C54" s="89"/>
@@ -52888,7 +52884,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" customHeight="1">
       <c r="A1" s="82" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -52902,13 +52898,13 @@
     <row r="2" spans="1:9" ht="16" customHeight="1">
       <c r="A2" s="71"/>
       <c r="B2" s="95" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C2" s="95"/>
       <c r="D2" s="95"/>
       <c r="E2" s="95"/>
       <c r="F2" s="92" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="G2" s="95"/>
       <c r="H2" s="95"/>
@@ -52917,28 +52913,28 @@
     <row r="3" spans="1:9" ht="30">
       <c r="A3" s="49"/>
       <c r="B3" s="41" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="H3" s="41" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -53004,16 +53000,16 @@
         <v>13</v>
       </c>
       <c r="B6" s="64" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C6" s="64" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D6" s="64" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="E6" s="50" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F6" s="64">
         <v>4241.1027974611998</v>
@@ -54422,7 +54418,7 @@
     </row>
     <row r="55" spans="1:9" ht="82.5" customHeight="1">
       <c r="A55" s="88" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="B55" s="89"/>
       <c r="C55" s="89"/>
@@ -54464,7 +54460,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="82" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -54476,37 +54472,37 @@
     <row r="2" spans="1:7">
       <c r="A2" s="49"/>
       <c r="B2" s="92" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C2" s="96"/>
       <c r="D2" s="92" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="E2" s="96"/>
       <c r="F2" s="92" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="G2" s="96"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="72"/>
       <c r="B3" s="41" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C3" s="41" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="E3" s="41" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="F3" s="41" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="G3" s="41" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -54517,19 +54513,19 @@
         <v>3347</v>
       </c>
       <c r="C4" s="73" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D4" s="73">
         <v>9139</v>
       </c>
       <c r="E4" s="73" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F4" s="74">
         <v>22957.531332988299</v>
       </c>
       <c r="G4" s="75" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -54560,10 +54556,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C6" s="76" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="D6" s="59">
         <v>6138.0901746155896</v>
@@ -55684,7 +55680,7 @@
     </row>
     <row r="55" spans="1:7" ht="80.25" customHeight="1">
       <c r="A55" s="88" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B55" s="89"/>
       <c r="C55" s="89"/>

</xml_diff>

<commit_message>
links to graph data under each graph
</commit_message>
<xml_diff>
--- a/data/DataforDownload.xlsx
+++ b/data/DataforDownload.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="43920" windowHeight="26360" tabRatio="821"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25280" windowHeight="26420" tabRatio="821"/>
   </bookViews>
   <sheets>
     <sheet name="1 Enroll.TwoYear" sheetId="6" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="6 Fund.TotalChange" sheetId="11" r:id="rId6"/>
     <sheet name="7 Fund.PerStudent" sheetId="12" r:id="rId7"/>
     <sheet name="8 Tuition.Change" sheetId="13" r:id="rId8"/>
-    <sheet name="9 Tuition.Tuition&amp;Rank" sheetId="14" r:id="rId9"/>
+    <sheet name="9 Tuition.TuitionandRank" sheetId="14" r:id="rId9"/>
     <sheet name="10 Annual Data" sheetId="1" r:id="rId10"/>
     <sheet name="11 Nonannual Data" sheetId="2" r:id="rId11"/>
     <sheet name="12 Sources" sheetId="3" r:id="rId12"/>
@@ -44922,7 +44922,7 @@
   <dimension ref="A1:P107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -54450,7 +54450,7 @@
   <dimension ref="A1:G55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>